<commit_message>
N-CTU PARA CONFIG Finish
</commit_message>
<xml_diff>
--- a/build-N-XTU-Desktop_Qt_5_8_0_MinGW_32bit-Debug/2018-10-25.xlsx
+++ b/build-N-XTU-Desktop_Qt_5_8_0_MinGW_32bit-Debug/2018-10-25.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>STATUS</t>
   </si>
@@ -57,11 +57,51 @@
     <t>TIME</t>
   </si>
   <si>
+    <t>000B57FFFEF609E3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>PASS</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>000B57FFFEF609E3</t>
+    <t>129.733 mA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20.135 mA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.007 mA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PASS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000B57FFFEF609E6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>121.584 mA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20.332 mA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.013 mA</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -70,18 +110,6 @@
   </si>
   <si>
     <t>0x0000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>129.667 mA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>20.133 mA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.009 mA</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -465,9 +493,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
@@ -528,16 +558,16 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>14</v>
-      </c>
       <c r="C2" s="4">
-        <v>-45</v>
+        <v>-46</v>
       </c>
       <c r="D2" s="5">
-        <v>1</v>
+        <v>0.999</v>
       </c>
       <c r="E2" s="4">
         <v>-45</v>
@@ -555,16 +585,57 @@
         <v>19</v>
       </c>
       <c r="J2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M2" s="6">
-        <v>43398.384942129633</v>
+        <v>43398.388136574074</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="4">
+        <v>-55</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0.99199999999999999</v>
+      </c>
+      <c r="E3" s="4">
+        <v>-55</v>
+      </c>
+      <c r="F3" s="5">
+        <v>1</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" s="6">
+        <v>43398.572187500002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>